<commit_message>
[QRS detection] OpenMP introduced
* Change:
  - Median and box filter are the most consuming parts
    of the program, so they are parallelized with OMP.

* Note:
  - On Intel(R) Core(TM) i5-3210M CPU with two physical
    cores speedup are showen below:
      - BoxFilter    2.28x speedup
      - MedianFilter 2.85x speedup
      - Total time   2.50x speedup

Signed-off-by: Dusan Kostic <kostic.dusan1990@gmail.com>
</commit_message>
<xml_diff>
--- a/QRS_report.xlsx
+++ b/QRS_report.xlsx
@@ -25,7 +25,7 @@
     <t>Date and time:</t>
   </si>
   <si>
-    <t>2014-07-27 19:58</t>
+    <t>2014-08-02 12:53</t>
   </si>
   <si>
     <t>Number of tests</t>
@@ -579,16 +579,16 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.421637021355784</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -613,13 +613,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -630,16 +630,16 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F15">
-        <v>0.421637021355784</v>
+        <v>1.82878222991269</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -647,16 +647,16 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>573</v>
+        <v>224</v>
       </c>
       <c r="D16">
-        <v>554</v>
+        <v>222</v>
       </c>
       <c r="E16">
-        <v>620</v>
+        <v>231</v>
       </c>
       <c r="F16">
-        <v>22.9482509621588</v>
+        <v>2.64365067451978</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -664,16 +664,16 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>623</v>
+        <v>250</v>
       </c>
       <c r="D17">
-        <v>604</v>
+        <v>248</v>
       </c>
       <c r="E17">
-        <v>670</v>
+        <v>256</v>
       </c>
       <c r="F17">
-        <v>22.8823075759417</v>
+        <v>2.60128173535022</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -681,16 +681,16 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.948683298050514</v>
       </c>
     </row>
     <row r="19" spans="2:6">
@@ -698,16 +698,16 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>2.20100986922922</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -715,16 +715,16 @@
         <v>21</v>
       </c>
       <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
         <v>17</v>
       </c>
-      <c r="D20">
-        <v>17</v>
-      </c>
-      <c r="E20">
-        <v>22</v>
-      </c>
       <c r="F20">
-        <v>1.54919333848297</v>
+        <v>0.421637021355784</v>
       </c>
     </row>
     <row r="21" spans="2:6">
@@ -749,16 +749,16 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>678</v>
+        <v>306</v>
       </c>
       <c r="D22">
-        <v>659</v>
+        <v>300</v>
       </c>
       <c r="E22">
-        <v>725</v>
+        <v>309</v>
       </c>
       <c r="F22">
-        <v>23.6664319237185</v>
+        <v>2.85968141193696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>